<commit_message>
Updated the UI for Course Management and fixed bugs
</commit_message>
<xml_diff>
--- a/Academic_data.xlsx
+++ b/Academic_data.xlsx
@@ -19,21 +19,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <x:si>
-    <x:t>아이디</x:t>
-  </x:si>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <x:si>
     <x:t>이름</x:t>
   </x:si>
   <x:si>
+    <x:t>최소언</x:t>
+  </x:si>
+  <x:si>
+    <x:t>직원번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주민등록번호</x:t>
+  </x:si>
+  <x:si>
     <x:t>비밀번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>3456789</x:t>
+  </x:si>
+  <x:si>
+    <x:t>thdjs07</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:numFmts count="0"/>
   <x:fonts count="6">
     <x:font>
       <x:name val="맑은 고딕"/>
@@ -399,35 +415,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="A1:C2"/>
+  <x:dimension ref="A1:D2"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="A3" activeCellId="0" sqref="A3:A3"/>
+      <x:selection activeCell="B3" activeCellId="0" sqref="B3:B3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.39999999999999857891"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
-      <x:c r="A1" t="s">
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" t="s" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B1" t="s" s="0">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C1" t="s">
+      <x:c r="C1" t="s" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D1" t="s" s="0">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="0">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B2" t="s" s="0">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
-      <x:c r="A2">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="B2">
+      <x:c r="C2" s="0">
         <x:v>123456789</x:v>
+      </x:c>
+      <x:c r="D2" t="s" s="0">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69999998807907104492" right="0.69999998807907104492" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
+  <x:pageMargins left="0.69972223043441772461" right="0.69972223043441772461" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>